<commit_message>
fix forms and translations
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/change_hoh.xlsx
+++ b/xforms/xlsforms/change_hoh.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="113">
   <si>
     <t>type</t>
   </si>
@@ -349,6 +349,12 @@
   </si>
   <si>
     <t>no-calendar</t>
+  </si>
+  <si>
+    <t>. &lt; today() and . &gt;${earliestDate}</t>
+  </si>
+  <si>
+    <t>Date of change of HoH can not be in the future or before ${earliestDate}</t>
   </si>
 </sst>
 </file>
@@ -853,7 +859,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
+      <selection pane="bottomRight" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75"/>
@@ -1186,7 +1192,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="13.5" thickTop="1">
+    <row r="15" spans="1:17" ht="39" thickTop="1">
       <c r="A15" s="13" t="s">
         <v>24</v>
       </c>
@@ -1198,6 +1204,12 @@
       </c>
       <c r="D15" s="13" t="s">
         <v>39</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>112</v>
       </c>
       <c r="H15" s="13" t="b">
         <v>1</v>

</xml_diff>